<commit_message>
Added algebraic rate names to Initialize.xlsx.  Modified get_data_dictionary.m to add rate names to data_dictionary.  Replaced xlsread with readtable for cross-platform compatibility.  Added calculate_rates.m for post-simulation rate calculation.
</commit_message>
<xml_diff>
--- a/Initialize.xlsx
+++ b/Initialize.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raor21/Documents/Projects/GitRepo/covid19_qsp_model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggene\Projects\covid19-immune-model-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63104FA1-3C73-804E-92AA-98486151E5C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5960AAF9-3E78-41F5-91AE-F7A9191F061E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{95AB0F38-69CF-4F4F-AFB9-30747DAFBDEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{95AB0F38-69CF-4F4F-AFB9-30747DAFBDEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
-    <sheet name="IC" sheetId="2" r:id="rId2"/>
+    <sheet name="Rates" sheetId="3" r:id="rId2"/>
+    <sheet name="IC" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="659">
   <si>
     <t>A_V</t>
   </si>
@@ -1664,12 +1675,354 @@
   </si>
   <si>
     <t>cells/uL</t>
+  </si>
+  <si>
+    <t>tr_TNFa</t>
+  </si>
+  <si>
+    <t>tr_IL6</t>
+  </si>
+  <si>
+    <t>tr_IL1b</t>
+  </si>
+  <si>
+    <t>tr_IFNb</t>
+  </si>
+  <si>
+    <t>tr_IFNg</t>
+  </si>
+  <si>
+    <t>tr_IL2</t>
+  </si>
+  <si>
+    <t>tr_IL12</t>
+  </si>
+  <si>
+    <t>tr_IL17</t>
+  </si>
+  <si>
+    <t>tr_IL10</t>
+  </si>
+  <si>
+    <t>tr_TGFb</t>
+  </si>
+  <si>
+    <t>tr_GMCSF</t>
+  </si>
+  <si>
+    <t>tr_SPD</t>
+  </si>
+  <si>
+    <t>tr_FER</t>
+  </si>
+  <si>
+    <t>tr_pDC</t>
+  </si>
+  <si>
+    <t>tr_M1</t>
+  </si>
+  <si>
+    <t>tr_N</t>
+  </si>
+  <si>
+    <t>tr_Th1</t>
+  </si>
+  <si>
+    <t>tr_Th17</t>
+  </si>
+  <si>
+    <t>tr_CTL</t>
+  </si>
+  <si>
+    <t>tr_Treg</t>
+  </si>
+  <si>
+    <t>prod_virus_shedding</t>
+  </si>
+  <si>
+    <t>virus_endocytosis</t>
+  </si>
+  <si>
+    <t>innate_clearance</t>
+  </si>
+  <si>
+    <t>deg_virus</t>
+  </si>
+  <si>
+    <t>ab_clearance</t>
+  </si>
+  <si>
+    <t>damage_cyt_AT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">damage_ROS_AT2 </t>
+  </si>
+  <si>
+    <t>growth_AT2</t>
+  </si>
+  <si>
+    <t>deg_AT2</t>
+  </si>
+  <si>
+    <t>diff_AT2</t>
+  </si>
+  <si>
+    <t>kill_CTL_I</t>
+  </si>
+  <si>
+    <t>deg_I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">growth_AT1 </t>
+  </si>
+  <si>
+    <t>damage_ROS_AT1</t>
+  </si>
+  <si>
+    <t>deg_AT1</t>
+  </si>
+  <si>
+    <t>deg_dAT1</t>
+  </si>
+  <si>
+    <t>deg_dAT2</t>
+  </si>
+  <si>
+    <t>act_pDC_TNFa</t>
+  </si>
+  <si>
+    <t>act_pDC_IFNg</t>
+  </si>
+  <si>
+    <t>act_pDC_IL6</t>
+  </si>
+  <si>
+    <t>act_pDC_GMCSF</t>
+  </si>
+  <si>
+    <t>inh_pDC_IL10</t>
+  </si>
+  <si>
+    <t>act_M1_TNFa</t>
+  </si>
+  <si>
+    <t>act_M1_GMCSF</t>
+  </si>
+  <si>
+    <t>act_M1_IFNg</t>
+  </si>
+  <si>
+    <t>inh_M1_IL10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">act_N_IFNg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">act_N_TNFa </t>
+  </si>
+  <si>
+    <t>act_N_GMCSF</t>
+  </si>
+  <si>
+    <t>rec_N_IL17c</t>
+  </si>
+  <si>
+    <t>act_Th1_IL12</t>
+  </si>
+  <si>
+    <t>act_Th1_IFNg</t>
+  </si>
+  <si>
+    <t>inh_Th1_IL10_TGFb</t>
+  </si>
+  <si>
+    <t>diff_Th1_Th17</t>
+  </si>
+  <si>
+    <t>diff_Th1_Treg</t>
+  </si>
+  <si>
+    <t>inh_Th17</t>
+  </si>
+  <si>
+    <t>act_TH17_TGFb</t>
+  </si>
+  <si>
+    <t>act_Th17_IL6</t>
+  </si>
+  <si>
+    <t>act_Th17_IL1b</t>
+  </si>
+  <si>
+    <t>act_CTL_IFNb</t>
+  </si>
+  <si>
+    <t>act_CTL_IL12</t>
+  </si>
+  <si>
+    <t>act_CTL_IFNg</t>
+  </si>
+  <si>
+    <t>act_Treg_IL2</t>
+  </si>
+  <si>
+    <t>act_Treg_TGFb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liver_CRP </t>
+  </si>
+  <si>
+    <t>prod_CRP_liver</t>
+  </si>
+  <si>
+    <t>tr_CRP</t>
+  </si>
+  <si>
+    <t>prod_CRP_blood</t>
+  </si>
+  <si>
+    <t>prod_tnf_dat1</t>
+  </si>
+  <si>
+    <t>prod_tnf_i</t>
+  </si>
+  <si>
+    <t>prod_tnf_dat2</t>
+  </si>
+  <si>
+    <t>prod_tnf_m1</t>
+  </si>
+  <si>
+    <t>prod_tnf_th1</t>
+  </si>
+  <si>
+    <t>prod_tnf_th17</t>
+  </si>
+  <si>
+    <t>deg_tnf</t>
+  </si>
+  <si>
+    <t>prod_il6_dat1</t>
+  </si>
+  <si>
+    <t>prod_il6_i</t>
+  </si>
+  <si>
+    <t>prod_il6_dat2</t>
+  </si>
+  <si>
+    <t>prod_il6_m1</t>
+  </si>
+  <si>
+    <t>prod_il6_th17</t>
+  </si>
+  <si>
+    <t>prod_il6_neu</t>
+  </si>
+  <si>
+    <t>deg_il6</t>
+  </si>
+  <si>
+    <t>prod_il1b_dat1</t>
+  </si>
+  <si>
+    <t>prod_il1b_i</t>
+  </si>
+  <si>
+    <t>prod_il1b_dat2</t>
+  </si>
+  <si>
+    <t>prod_il1b_m1</t>
+  </si>
+  <si>
+    <t>prod_il1b_dc</t>
+  </si>
+  <si>
+    <t>deg_il1b</t>
+  </si>
+  <si>
+    <t>prod_ifng_dc</t>
+  </si>
+  <si>
+    <t>prod_ifng_th1</t>
+  </si>
+  <si>
+    <t>prod_ifng_ctl</t>
+  </si>
+  <si>
+    <t>del_ifng</t>
+  </si>
+  <si>
+    <t>prod_ifnb_i</t>
+  </si>
+  <si>
+    <t>prod_ifnb_dc</t>
+  </si>
+  <si>
+    <t>del_ifnb</t>
+  </si>
+  <si>
+    <t>prod_il2_dc</t>
+  </si>
+  <si>
+    <t>prod_il2_th1</t>
+  </si>
+  <si>
+    <t>deg_il2</t>
+  </si>
+  <si>
+    <t>prod_il12_m1</t>
+  </si>
+  <si>
+    <t>prod_il12_dc</t>
+  </si>
+  <si>
+    <t>deg_il12</t>
+  </si>
+  <si>
+    <t>prod_il17_th17</t>
+  </si>
+  <si>
+    <t>prod_il17_ctl</t>
+  </si>
+  <si>
+    <t>deg_il17</t>
+  </si>
+  <si>
+    <t>prod_il10_treg</t>
+  </si>
+  <si>
+    <t>deg_il10</t>
+  </si>
+  <si>
+    <t>prod_tgfb_th17</t>
+  </si>
+  <si>
+    <t>prod_tgfb_treg</t>
+  </si>
+  <si>
+    <t>deg_tgfb</t>
+  </si>
+  <si>
+    <t>prod_gmcsf_m1</t>
+  </si>
+  <si>
+    <t>prod_gmcsf_th1</t>
+  </si>
+  <si>
+    <t>prod_gmcsf_th17</t>
+  </si>
+  <si>
+    <t>deg_gmcsf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1759,7 +2112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1775,13 +2128,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2098,20 +2456,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF1439E-DB2C-7B45-8415-667380488B1F}">
   <dimension ref="A1:E231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="62.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.19921875" customWidth="1"/>
+    <col min="3" max="3" width="62.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.296875" customWidth="1"/>
+    <col min="5" max="5" width="26.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2124,11 +2482,11 @@
       <c r="D1" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2141,9 +2499,9 @@
       <c r="D2" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2157,9 +2515,9 @@
       <c r="D3" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="16"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -2172,9 +2530,9 @@
       <c r="D4" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E4" s="15"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="16"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2187,9 +2545,9 @@
       <c r="D5" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="E5" s="15"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -2202,9 +2560,9 @@
       <c r="D6" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2217,9 +2575,9 @@
       <c r="D7" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -2232,9 +2590,9 @@
       <c r="D8" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2247,9 +2605,9 @@
       <c r="D9" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E9" s="15"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -2262,9 +2620,9 @@
       <c r="D10" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -2277,9 +2635,9 @@
       <c r="D11" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E11" s="15"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -2293,9 +2651,9 @@
       <c r="D12" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -2308,9 +2666,9 @@
       <c r="D13" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -2323,9 +2681,9 @@
       <c r="D14" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -2338,9 +2696,9 @@
       <c r="D15" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -2353,9 +2711,9 @@
       <c r="D16" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -2368,9 +2726,9 @@
       <c r="D17" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -2383,9 +2741,9 @@
       <c r="D18" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="16"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -2398,9 +2756,9 @@
       <c r="D19" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -2413,9 +2771,9 @@
       <c r="D20" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -2428,9 +2786,9 @@
       <c r="D21" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="16"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -2443,9 +2801,9 @@
       <c r="D22" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E22" s="15"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -2458,9 +2816,9 @@
       <c r="D23" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -2473,9 +2831,9 @@
       <c r="D24" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -2489,9 +2847,9 @@
       <c r="D25" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E25" s="15"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -2504,9 +2862,9 @@
       <c r="D26" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E26" s="15"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -2520,9 +2878,9 @@
       <c r="D27" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E27" s="16"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
@@ -2535,9 +2893,9 @@
       <c r="D28" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E28" s="15"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E28" s="16"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
@@ -2551,9 +2909,9 @@
       <c r="D29" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="16"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
@@ -2566,9 +2924,9 @@
       <c r="D30" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E30" s="15"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="16"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>308</v>
       </c>
@@ -2581,9 +2939,9 @@
       <c r="D31" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="E31" s="15"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="16"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>309</v>
       </c>
@@ -2596,9 +2954,9 @@
       <c r="D32" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="E32" s="15"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="16"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>28</v>
       </c>
@@ -2611,11 +2969,11 @@
       <c r="D33" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="17" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>29</v>
       </c>
@@ -2628,9 +2986,9 @@
       <c r="D34" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="E34" s="16"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E34" s="17"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>30</v>
       </c>
@@ -2643,9 +3001,9 @@
       <c r="D35" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E35" s="16"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E35" s="17"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>31</v>
       </c>
@@ -2658,9 +3016,9 @@
       <c r="D36" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E36" s="16"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E36" s="17"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>32</v>
       </c>
@@ -2673,9 +3031,9 @@
       <c r="D37" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E37" s="16"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E37" s="17"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>33</v>
       </c>
@@ -2688,9 +3046,9 @@
       <c r="D38" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E38" s="16"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E38" s="17"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>34</v>
       </c>
@@ -2703,9 +3061,9 @@
       <c r="D39" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E39" s="16"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E39" s="17"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>35</v>
       </c>
@@ -2718,9 +3076,9 @@
       <c r="D40" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E40" s="16"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E40" s="17"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>36</v>
       </c>
@@ -2733,9 +3091,9 @@
       <c r="D41" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E41" s="16"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E41" s="17"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>37</v>
       </c>
@@ -2748,9 +3106,9 @@
       <c r="D42" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E42" s="16"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="17"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>40</v>
       </c>
@@ -2763,11 +3121,11 @@
       <c r="D43" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="16" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>41</v>
       </c>
@@ -2780,9 +3138,9 @@
       <c r="D44" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E44" s="15"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E44" s="16"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>42</v>
       </c>
@@ -2795,9 +3153,9 @@
       <c r="D45" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E45" s="15"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E45" s="16"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>43</v>
       </c>
@@ -2810,9 +3168,9 @@
       <c r="D46" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E46" s="15"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E46" s="16"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>251</v>
       </c>
@@ -2825,9 +3183,9 @@
       <c r="D47" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E47" s="15"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E47" s="16"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>44</v>
       </c>
@@ -2840,9 +3198,9 @@
       <c r="D48" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E48" s="15"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E48" s="16"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>45</v>
       </c>
@@ -2855,9 +3213,9 @@
       <c r="D49" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E49" s="15"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E49" s="16"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>252</v>
       </c>
@@ -2870,9 +3228,9 @@
       <c r="D50" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E50" s="15"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E50" s="16"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>46</v>
       </c>
@@ -2885,9 +3243,9 @@
       <c r="D51" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E51" s="15"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E51" s="16"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>47</v>
       </c>
@@ -2900,9 +3258,9 @@
       <c r="D52" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E52" s="15"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E52" s="16"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>48</v>
       </c>
@@ -2915,9 +3273,9 @@
       <c r="D53" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E53" s="15"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E53" s="16"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>49</v>
       </c>
@@ -2930,9 +3288,9 @@
       <c r="D54" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E54" s="15"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E54" s="16"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>50</v>
       </c>
@@ -2945,9 +3303,9 @@
       <c r="D55" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E55" s="15"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E55" s="16"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>51</v>
       </c>
@@ -2960,9 +3318,9 @@
       <c r="D56" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E56" s="15"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E56" s="16"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>52</v>
       </c>
@@ -2975,9 +3333,9 @@
       <c r="D57" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E57" s="15"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E57" s="16"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>53</v>
       </c>
@@ -2990,9 +3348,9 @@
       <c r="D58" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E58" s="15"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E58" s="16"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>54</v>
       </c>
@@ -3005,9 +3363,9 @@
       <c r="D59" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E59" s="15"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E59" s="16"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>55</v>
       </c>
@@ -3020,9 +3378,9 @@
       <c r="D60" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E60" s="15"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E60" s="16"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>310</v>
       </c>
@@ -3035,11 +3393,11 @@
       <c r="D61" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E61" s="17" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>56</v>
       </c>
@@ -3052,9 +3410,9 @@
       <c r="D62" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="E62" s="16"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E62" s="17"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>57</v>
       </c>
@@ -3067,9 +3425,9 @@
       <c r="D63" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E63" s="16"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E63" s="17"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
         <v>58</v>
       </c>
@@ -3082,9 +3440,9 @@
       <c r="D64" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E64" s="16"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E64" s="17"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
         <v>194</v>
       </c>
@@ -3097,9 +3455,9 @@
       <c r="D65" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E65" s="16"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E65" s="17"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
         <v>195</v>
       </c>
@@ -3112,9 +3470,9 @@
       <c r="D66" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E66" s="16"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E66" s="17"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
         <v>59</v>
       </c>
@@ -3127,9 +3485,9 @@
       <c r="D67" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E67" s="16"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E67" s="17"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
         <v>60</v>
       </c>
@@ -3142,9 +3500,9 @@
       <c r="D68" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E68" s="16"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E68" s="17"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
         <v>61</v>
       </c>
@@ -3157,9 +3515,9 @@
       <c r="D69" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E69" s="16"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E69" s="17"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
         <v>62</v>
       </c>
@@ -3172,9 +3530,9 @@
       <c r="D70" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E70" s="16"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E70" s="17"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>63</v>
       </c>
@@ -3187,9 +3545,9 @@
       <c r="D71" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E71" s="16"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E71" s="17"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>64</v>
       </c>
@@ -3202,11 +3560,11 @@
       <c r="D72" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E72" s="15" t="s">
+      <c r="E72" s="16" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>65</v>
       </c>
@@ -3219,9 +3577,9 @@
       <c r="D73" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E73" s="15"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E73" s="16"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>66</v>
       </c>
@@ -3234,9 +3592,9 @@
       <c r="D74" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E74" s="15"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E74" s="16"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>67</v>
       </c>
@@ -3249,9 +3607,9 @@
       <c r="D75" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E75" s="15"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E75" s="16"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>68</v>
       </c>
@@ -3264,9 +3622,9 @@
       <c r="D76" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E76" s="15"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E76" s="16"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>69</v>
       </c>
@@ -3279,9 +3637,9 @@
       <c r="D77" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E77" s="15"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E77" s="16"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>70</v>
       </c>
@@ -3294,9 +3652,9 @@
       <c r="D78" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E78" s="15"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E78" s="16"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>71</v>
       </c>
@@ -3309,9 +3667,9 @@
       <c r="D79" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E79" s="15"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E79" s="16"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>72</v>
       </c>
@@ -3324,9 +3682,9 @@
       <c r="D80" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E80" s="15"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E80" s="16"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>73</v>
       </c>
@@ -3339,9 +3697,9 @@
       <c r="D81" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E81" s="15"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E81" s="16"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>74</v>
       </c>
@@ -3354,9 +3712,9 @@
       <c r="D82" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E82" s="15"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E82" s="16"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>75</v>
       </c>
@@ -3369,9 +3727,9 @@
       <c r="D83" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E83" s="15"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E83" s="16"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>76</v>
       </c>
@@ -3384,9 +3742,9 @@
       <c r="D84" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E84" s="15"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E84" s="16"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>77</v>
       </c>
@@ -3399,9 +3757,9 @@
       <c r="D85" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E85" s="15"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E85" s="16"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>78</v>
       </c>
@@ -3414,9 +3772,9 @@
       <c r="D86" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E86" s="15"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E86" s="16"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
         <v>79</v>
       </c>
@@ -3429,11 +3787,11 @@
       <c r="D87" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="E87" s="16" t="s">
+      <c r="E87" s="17" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="9" t="s">
         <v>80</v>
       </c>
@@ -3446,9 +3804,9 @@
       <c r="D88" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E88" s="16"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E88" s="17"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
         <v>81</v>
       </c>
@@ -3461,9 +3819,9 @@
       <c r="D89" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E89" s="16"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E89" s="17"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
         <v>82</v>
       </c>
@@ -3476,9 +3834,9 @@
       <c r="D90" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E90" s="16"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E90" s="17"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="9" t="s">
         <v>83</v>
       </c>
@@ -3491,9 +3849,9 @@
       <c r="D91" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E91" s="16"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E91" s="17"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="9" t="s">
         <v>84</v>
       </c>
@@ -3506,9 +3864,9 @@
       <c r="D92" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E92" s="16"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E92" s="17"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
         <v>85</v>
       </c>
@@ -3521,9 +3879,9 @@
       <c r="D93" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E93" s="16"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E93" s="17"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
         <v>86</v>
       </c>
@@ -3536,9 +3894,9 @@
       <c r="D94" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E94" s="16"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E94" s="17"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
         <v>87</v>
       </c>
@@ -3551,9 +3909,9 @@
       <c r="D95" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E95" s="16"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E95" s="17"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
         <v>88</v>
       </c>
@@ -3566,9 +3924,9 @@
       <c r="D96" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E96" s="16"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E96" s="17"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
         <v>89</v>
       </c>
@@ -3581,9 +3939,9 @@
       <c r="D97" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E97" s="16"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E97" s="17"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>90</v>
       </c>
@@ -3596,11 +3954,11 @@
       <c r="D98" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E98" s="15" t="s">
+      <c r="E98" s="16" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>91</v>
       </c>
@@ -3613,9 +3971,9 @@
       <c r="D99" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E99" s="15"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E99" s="16"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>92</v>
       </c>
@@ -3628,9 +3986,9 @@
       <c r="D100" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E100" s="15"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E100" s="16"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>93</v>
       </c>
@@ -3643,9 +4001,9 @@
       <c r="D101" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E101" s="15"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E101" s="16"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>94</v>
       </c>
@@ -3658,9 +4016,9 @@
       <c r="D102" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E102" s="15"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E102" s="16"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>95</v>
       </c>
@@ -3673,9 +4031,9 @@
       <c r="D103" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E103" s="15"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E103" s="16"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>96</v>
       </c>
@@ -3688,9 +4046,9 @@
       <c r="D104" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E104" s="15"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E104" s="16"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>97</v>
       </c>
@@ -3703,9 +4061,9 @@
       <c r="D105" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E105" s="15"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E105" s="16"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>98</v>
       </c>
@@ -3718,9 +4076,9 @@
       <c r="D106" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E106" s="15"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E106" s="16"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>99</v>
       </c>
@@ -3733,9 +4091,9 @@
       <c r="D107" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E107" s="15"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E107" s="16"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>100</v>
       </c>
@@ -3748,9 +4106,9 @@
       <c r="D108" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E108" s="15"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E108" s="16"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>101</v>
       </c>
@@ -3763,9 +4121,9 @@
       <c r="D109" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E109" s="15"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E109" s="16"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>102</v>
       </c>
@@ -3778,9 +4136,9 @@
       <c r="D110" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E110" s="15"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E110" s="16"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="9" t="s">
         <v>103</v>
       </c>
@@ -3793,11 +4151,11 @@
       <c r="D111" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="E111" s="16" t="s">
+      <c r="E111" s="17" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="9" t="s">
         <v>104</v>
       </c>
@@ -3810,9 +4168,9 @@
       <c r="D112" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E112" s="16"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E112" s="17"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="9" t="s">
         <v>105</v>
       </c>
@@ -3825,9 +4183,9 @@
       <c r="D113" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E113" s="16"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E113" s="17"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="9" t="s">
         <v>106</v>
       </c>
@@ -3840,9 +4198,9 @@
       <c r="D114" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E114" s="16"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E114" s="17"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="9" t="s">
         <v>107</v>
       </c>
@@ -3855,9 +4213,9 @@
       <c r="D115" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E115" s="16"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E115" s="17"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="9" t="s">
         <v>108</v>
       </c>
@@ -3870,9 +4228,9 @@
       <c r="D116" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E116" s="16"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E116" s="17"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="9" t="s">
         <v>109</v>
       </c>
@@ -3885,9 +4243,9 @@
       <c r="D117" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E117" s="16"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E117" s="17"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="9" t="s">
         <v>110</v>
       </c>
@@ -3900,9 +4258,9 @@
       <c r="D118" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E118" s="16"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E118" s="17"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>111</v>
       </c>
@@ -3915,11 +4273,11 @@
       <c r="D119" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="E119" s="15" t="s">
+      <c r="E119" s="16" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>112</v>
       </c>
@@ -3932,9 +4290,9 @@
       <c r="D120" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="E120" s="15"/>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E120" s="16"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>113</v>
       </c>
@@ -3947,9 +4305,9 @@
       <c r="D121" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E121" s="15"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E121" s="16"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>114</v>
       </c>
@@ -3962,9 +4320,9 @@
       <c r="D122" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="E122" s="15"/>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E122" s="16"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>115</v>
       </c>
@@ -3977,9 +4335,9 @@
       <c r="D123" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="E123" s="15"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E123" s="16"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>116</v>
       </c>
@@ -3992,9 +4350,9 @@
       <c r="D124" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E124" s="15"/>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E124" s="16"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>250</v>
       </c>
@@ -4007,9 +4365,9 @@
       <c r="D125" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="E125" s="15"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E125" s="16"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>331</v>
       </c>
@@ -4022,9 +4380,9 @@
       <c r="D126" s="12" t="s">
         <v>519</v>
       </c>
-      <c r="E126" s="15"/>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E126" s="16"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>332</v>
       </c>
@@ -4037,9 +4395,9 @@
       <c r="D127" s="12" t="s">
         <v>519</v>
       </c>
-      <c r="E127" s="15"/>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E127" s="16"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>311</v>
       </c>
@@ -4052,9 +4410,9 @@
       <c r="D128" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="E128" s="15"/>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E128" s="16"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>312</v>
       </c>
@@ -4067,9 +4425,9 @@
       <c r="D129" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="E129" s="15"/>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E129" s="16"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>313</v>
       </c>
@@ -4082,9 +4440,9 @@
       <c r="D130" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="E130" s="15"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E130" s="16"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>314</v>
       </c>
@@ -4097,9 +4455,9 @@
       <c r="D131" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="E131" s="15"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E131" s="16"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>315</v>
       </c>
@@ -4112,9 +4470,9 @@
       <c r="D132" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="E132" s="15"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E132" s="16"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>316</v>
       </c>
@@ -4127,9 +4485,9 @@
       <c r="D133" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="E133" s="15"/>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E133" s="16"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>317</v>
       </c>
@@ -4142,9 +4500,9 @@
       <c r="D134" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="E134" s="15"/>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E134" s="16"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>320</v>
       </c>
@@ -4157,9 +4515,9 @@
       <c r="D135" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="E135" s="15"/>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E135" s="16"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="9" t="s">
         <v>117</v>
       </c>
@@ -4172,11 +4530,11 @@
       <c r="D136" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="E136" s="16" t="s">
+      <c r="E136" s="17" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="9" t="s">
         <v>118</v>
       </c>
@@ -4189,9 +4547,9 @@
       <c r="D137" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E137" s="16"/>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E137" s="17"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="9" t="s">
         <v>119</v>
       </c>
@@ -4204,9 +4562,9 @@
       <c r="D138" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E138" s="16"/>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E138" s="17"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="9" t="s">
         <v>120</v>
       </c>
@@ -4219,9 +4577,9 @@
       <c r="D139" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E139" s="16"/>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E139" s="17"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="9" t="s">
         <v>121</v>
       </c>
@@ -4234,9 +4592,9 @@
       <c r="D140" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E140" s="16"/>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E140" s="17"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="9" t="s">
         <v>122</v>
       </c>
@@ -4249,9 +4607,9 @@
       <c r="D141" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E141" s="16"/>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E141" s="17"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="9" t="s">
         <v>123</v>
       </c>
@@ -4264,9 +4622,9 @@
       <c r="D142" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E142" s="16"/>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E142" s="17"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="9" t="s">
         <v>124</v>
       </c>
@@ -4279,9 +4637,9 @@
       <c r="D143" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E143" s="16"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E143" s="17"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="9" t="s">
         <v>125</v>
       </c>
@@ -4294,9 +4652,9 @@
       <c r="D144" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E144" s="16"/>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E144" s="17"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="9" t="s">
         <v>126</v>
       </c>
@@ -4309,9 +4667,9 @@
       <c r="D145" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E145" s="16"/>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E145" s="17"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="9" t="s">
         <v>127</v>
       </c>
@@ -4324,9 +4682,9 @@
       <c r="D146" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E146" s="16"/>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E146" s="17"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="9" t="s">
         <v>128</v>
       </c>
@@ -4339,9 +4697,9 @@
       <c r="D147" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E147" s="16"/>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E147" s="17"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="9" t="s">
         <v>129</v>
       </c>
@@ -4354,9 +4712,9 @@
       <c r="D148" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E148" s="16"/>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E148" s="17"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="9" t="s">
         <v>130</v>
       </c>
@@ -4369,9 +4727,9 @@
       <c r="D149" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E149" s="16"/>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E149" s="17"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="9" t="s">
         <v>131</v>
       </c>
@@ -4384,9 +4742,9 @@
       <c r="D150" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E150" s="16"/>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E150" s="17"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="9" t="s">
         <v>132</v>
       </c>
@@ -4399,9 +4757,9 @@
       <c r="D151" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E151" s="16"/>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E151" s="17"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="9" t="s">
         <v>133</v>
       </c>
@@ -4414,9 +4772,9 @@
       <c r="D152" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E152" s="16"/>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E152" s="17"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="9" t="s">
         <v>134</v>
       </c>
@@ -4429,9 +4787,9 @@
       <c r="D153" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E153" s="16"/>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E153" s="17"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="9" t="s">
         <v>135</v>
       </c>
@@ -4444,9 +4802,9 @@
       <c r="D154" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E154" s="16"/>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E154" s="17"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="9" t="s">
         <v>136</v>
       </c>
@@ -4459,9 +4817,9 @@
       <c r="D155" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E155" s="16"/>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E155" s="17"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="9" t="s">
         <v>137</v>
       </c>
@@ -4474,9 +4832,9 @@
       <c r="D156" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E156" s="16"/>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E156" s="17"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="9" t="s">
         <v>138</v>
       </c>
@@ -4489,9 +4847,9 @@
       <c r="D157" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E157" s="16"/>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E157" s="17"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="9" t="s">
         <v>139</v>
       </c>
@@ -4504,9 +4862,9 @@
       <c r="D158" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E158" s="16"/>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E158" s="17"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="9" t="s">
         <v>140</v>
       </c>
@@ -4519,9 +4877,9 @@
       <c r="D159" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E159" s="16"/>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E159" s="17"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="9" t="s">
         <v>141</v>
       </c>
@@ -4534,9 +4892,9 @@
       <c r="D160" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E160" s="16"/>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E160" s="17"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="9" t="s">
         <v>142</v>
       </c>
@@ -4549,9 +4907,9 @@
       <c r="D161" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E161" s="16"/>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E161" s="17"/>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="9" t="s">
         <v>143</v>
       </c>
@@ -4564,9 +4922,9 @@
       <c r="D162" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E162" s="16"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E162" s="17"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="9" t="s">
         <v>144</v>
       </c>
@@ -4579,9 +4937,9 @@
       <c r="D163" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E163" s="16"/>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E163" s="17"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="9" t="s">
         <v>145</v>
       </c>
@@ -4594,9 +4952,9 @@
       <c r="D164" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E164" s="16"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E164" s="17"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="9" t="s">
         <v>146</v>
       </c>
@@ -4609,9 +4967,9 @@
       <c r="D165" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E165" s="16"/>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E165" s="17"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="9" t="s">
         <v>147</v>
       </c>
@@ -4624,9 +4982,9 @@
       <c r="D166" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E166" s="16"/>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E166" s="17"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="9" t="s">
         <v>148</v>
       </c>
@@ -4639,9 +4997,9 @@
       <c r="D167" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E167" s="16"/>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E167" s="17"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="9" t="s">
         <v>149</v>
       </c>
@@ -4654,9 +5012,9 @@
       <c r="D168" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E168" s="16"/>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E168" s="17"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="9" t="s">
         <v>150</v>
       </c>
@@ -4669,9 +5027,9 @@
       <c r="D169" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E169" s="16"/>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E169" s="17"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="9" t="s">
         <v>151</v>
       </c>
@@ -4684,9 +5042,9 @@
       <c r="D170" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E170" s="16"/>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E170" s="17"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="9" t="s">
         <v>152</v>
       </c>
@@ -4699,9 +5057,9 @@
       <c r="D171" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E171" s="16"/>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E171" s="17"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="9" t="s">
         <v>153</v>
       </c>
@@ -4714,9 +5072,9 @@
       <c r="D172" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E172" s="16"/>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E172" s="17"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="9" t="s">
         <v>154</v>
       </c>
@@ -4729,9 +5087,9 @@
       <c r="D173" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E173" s="16"/>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E173" s="17"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="9" t="s">
         <v>155</v>
       </c>
@@ -4744,9 +5102,9 @@
       <c r="D174" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E174" s="16"/>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E174" s="17"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="9" t="s">
         <v>156</v>
       </c>
@@ -4759,9 +5117,9 @@
       <c r="D175" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E175" s="16"/>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E175" s="17"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="9" t="s">
         <v>157</v>
       </c>
@@ -4774,9 +5132,9 @@
       <c r="D176" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E176" s="16"/>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E176" s="17"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="9" t="s">
         <v>158</v>
       </c>
@@ -4789,9 +5147,9 @@
       <c r="D177" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E177" s="16"/>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E177" s="17"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="9" t="s">
         <v>159</v>
       </c>
@@ -4804,9 +5162,9 @@
       <c r="D178" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E178" s="16"/>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E178" s="17"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="9" t="s">
         <v>160</v>
       </c>
@@ -4819,9 +5177,9 @@
       <c r="D179" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E179" s="16"/>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E179" s="17"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="9" t="s">
         <v>161</v>
       </c>
@@ -4834,9 +5192,9 @@
       <c r="D180" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E180" s="16"/>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E180" s="17"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="9" t="s">
         <v>162</v>
       </c>
@@ -4849,9 +5207,9 @@
       <c r="D181" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E181" s="16"/>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E181" s="17"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="9" t="s">
         <v>163</v>
       </c>
@@ -4864,9 +5222,9 @@
       <c r="D182" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E182" s="16"/>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E182" s="17"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="9" t="s">
         <v>164</v>
       </c>
@@ -4879,9 +5237,9 @@
       <c r="D183" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E183" s="16"/>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E183" s="17"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="9" t="s">
         <v>165</v>
       </c>
@@ -4894,9 +5252,9 @@
       <c r="D184" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E184" s="16"/>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E184" s="17"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="9" t="s">
         <v>166</v>
       </c>
@@ -4909,9 +5267,9 @@
       <c r="D185" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E185" s="16"/>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E185" s="17"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="9" t="s">
         <v>167</v>
       </c>
@@ -4924,9 +5282,9 @@
       <c r="D186" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E186" s="16"/>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E186" s="17"/>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="9" t="s">
         <v>168</v>
       </c>
@@ -4939,9 +5297,9 @@
       <c r="D187" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E187" s="16"/>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E187" s="17"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="9" t="s">
         <v>169</v>
       </c>
@@ -4954,9 +5312,9 @@
       <c r="D188" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E188" s="16"/>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E188" s="17"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="9" t="s">
         <v>170</v>
       </c>
@@ -4969,9 +5327,9 @@
       <c r="D189" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E189" s="16"/>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E189" s="17"/>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="9" t="s">
         <v>171</v>
       </c>
@@ -4984,9 +5342,9 @@
       <c r="D190" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E190" s="16"/>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E190" s="17"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="9" t="s">
         <v>172</v>
       </c>
@@ -4999,9 +5357,9 @@
       <c r="D191" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E191" s="16"/>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E191" s="17"/>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="9" t="s">
         <v>173</v>
       </c>
@@ -5014,9 +5372,9 @@
       <c r="D192" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E192" s="16"/>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E192" s="17"/>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="9" t="s">
         <v>174</v>
       </c>
@@ -5029,9 +5387,9 @@
       <c r="D193" s="10" t="s">
         <v>519</v>
       </c>
-      <c r="E193" s="16"/>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E193" s="17"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="9" t="s">
         <v>175</v>
       </c>
@@ -5044,9 +5402,9 @@
       <c r="D194" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E194" s="16"/>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E194" s="17"/>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="9" t="s">
         <v>176</v>
       </c>
@@ -5059,9 +5417,9 @@
       <c r="D195" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E195" s="16"/>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E195" s="17"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="9" t="s">
         <v>321</v>
       </c>
@@ -5074,9 +5432,9 @@
       <c r="D196" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E196" s="16"/>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E196" s="17"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="9" t="s">
         <v>322</v>
       </c>
@@ -5089,9 +5447,9 @@
       <c r="D197" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E197" s="16"/>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E197" s="17"/>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="9" t="s">
         <v>323</v>
       </c>
@@ -5104,9 +5462,9 @@
       <c r="D198" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E198" s="16"/>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E198" s="17"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="9" t="s">
         <v>330</v>
       </c>
@@ -5119,9 +5477,9 @@
       <c r="D199" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E199" s="16"/>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E199" s="17"/>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="9" t="s">
         <v>324</v>
       </c>
@@ -5134,9 +5492,9 @@
       <c r="D200" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E200" s="16"/>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E200" s="17"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="9" t="s">
         <v>325</v>
       </c>
@@ -5149,9 +5507,9 @@
       <c r="D201" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E201" s="16"/>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E201" s="17"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="9" t="s">
         <v>326</v>
       </c>
@@ -5164,9 +5522,9 @@
       <c r="D202" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E202" s="16"/>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E202" s="17"/>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="9" t="s">
         <v>327</v>
       </c>
@@ -5179,9 +5537,9 @@
       <c r="D203" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E203" s="16"/>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E203" s="17"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="9" t="s">
         <v>328</v>
       </c>
@@ -5194,9 +5552,9 @@
       <c r="D204" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E204" s="16"/>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E204" s="17"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="9" t="s">
         <v>329</v>
       </c>
@@ -5209,9 +5567,9 @@
       <c r="D205" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="E205" s="16"/>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E205" s="17"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="3" t="s">
         <v>177</v>
       </c>
@@ -5224,11 +5582,11 @@
       <c r="D206" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E206" s="15" t="s">
+      <c r="E206" s="16" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="3" t="s">
         <v>178</v>
       </c>
@@ -5241,9 +5599,9 @@
       <c r="D207" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E207" s="15"/>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E207" s="16"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="3" t="s">
         <v>179</v>
       </c>
@@ -5256,9 +5614,9 @@
       <c r="D208" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E208" s="15"/>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E208" s="16"/>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="3" t="s">
         <v>180</v>
       </c>
@@ -5271,9 +5629,9 @@
       <c r="D209" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E209" s="15"/>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E209" s="16"/>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="3" t="s">
         <v>181</v>
       </c>
@@ -5286,9 +5644,9 @@
       <c r="D210" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E210" s="15"/>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E210" s="16"/>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="3" t="s">
         <v>182</v>
       </c>
@@ -5301,9 +5659,9 @@
       <c r="D211" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E211" s="15"/>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E211" s="16"/>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="3" t="s">
         <v>183</v>
       </c>
@@ -5316,9 +5674,9 @@
       <c r="D212" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E212" s="15"/>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E212" s="16"/>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="3" t="s">
         <v>184</v>
       </c>
@@ -5331,9 +5689,9 @@
       <c r="D213" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E213" s="15"/>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E213" s="16"/>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="3" t="s">
         <v>185</v>
       </c>
@@ -5346,9 +5704,9 @@
       <c r="D214" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E214" s="15"/>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E214" s="16"/>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="3" t="s">
         <v>186</v>
       </c>
@@ -5361,9 +5719,9 @@
       <c r="D215" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E215" s="15"/>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E215" s="16"/>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="3" t="s">
         <v>187</v>
       </c>
@@ -5376,9 +5734,9 @@
       <c r="D216" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E216" s="15"/>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E216" s="16"/>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="3" t="s">
         <v>188</v>
       </c>
@@ -5391,9 +5749,9 @@
       <c r="D217" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E217" s="15"/>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E217" s="16"/>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="3" t="s">
         <v>189</v>
       </c>
@@ -5406,9 +5764,9 @@
       <c r="D218" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E218" s="15"/>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E218" s="16"/>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="3" t="s">
         <v>193</v>
       </c>
@@ -5421,9 +5779,9 @@
       <c r="D219" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="E219" s="15"/>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E219" s="16"/>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="3" t="s">
         <v>243</v>
       </c>
@@ -5436,9 +5794,9 @@
       <c r="D220" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E220" s="15"/>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E220" s="16"/>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="3" t="s">
         <v>244</v>
       </c>
@@ -5451,9 +5809,9 @@
       <c r="D221" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E221" s="15"/>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E221" s="16"/>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="3" t="s">
         <v>245</v>
       </c>
@@ -5466,9 +5824,9 @@
       <c r="D222" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E222" s="15"/>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E222" s="16"/>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="3" t="s">
         <v>246</v>
       </c>
@@ -5481,9 +5839,9 @@
       <c r="D223" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E223" s="15"/>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E223" s="16"/>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="3" t="s">
         <v>247</v>
       </c>
@@ -5496,9 +5854,9 @@
       <c r="D224" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E224" s="15"/>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E224" s="16"/>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="3" t="s">
         <v>248</v>
       </c>
@@ -5511,9 +5869,9 @@
       <c r="D225" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E225" s="15"/>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E225" s="16"/>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="3" t="s">
         <v>249</v>
       </c>
@@ -5526,9 +5884,9 @@
       <c r="D226" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E226" s="15"/>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E226" s="16"/>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="9" t="s">
         <v>190</v>
       </c>
@@ -5541,11 +5899,11 @@
       <c r="D227" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="E227" s="16" t="s">
+      <c r="E227" s="17" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="9" t="s">
         <v>191</v>
       </c>
@@ -5558,9 +5916,9 @@
       <c r="D228" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="E228" s="16"/>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E228" s="17"/>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="9" t="s">
         <v>192</v>
       </c>
@@ -5573,9 +5931,9 @@
       <c r="D229" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="E229" s="16"/>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E229" s="17"/>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="3" t="s">
         <v>318</v>
       </c>
@@ -5590,7 +5948,7 @@
       </c>
       <c r="E230" s="11"/>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="3" t="s">
         <v>319</v>
       </c>
@@ -5607,16 +5965,16 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E33:E42"/>
+    <mergeCell ref="E1:E32"/>
+    <mergeCell ref="E43:E60"/>
+    <mergeCell ref="E72:E86"/>
+    <mergeCell ref="E98:E110"/>
     <mergeCell ref="E206:E226"/>
     <mergeCell ref="E227:E229"/>
     <mergeCell ref="E111:E118"/>
     <mergeCell ref="E87:E97"/>
     <mergeCell ref="E61:E71"/>
-    <mergeCell ref="E33:E42"/>
-    <mergeCell ref="E1:E32"/>
-    <mergeCell ref="E43:E60"/>
-    <mergeCell ref="E72:E86"/>
-    <mergeCell ref="E98:E110"/>
     <mergeCell ref="E119:E135"/>
     <mergeCell ref="E136:E205"/>
   </mergeCells>
@@ -5625,23 +5983,955 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2FD2B59-4E11-434A-BFD8-98DF25508CBA}">
+  <dimension ref="A1:C114"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.296875" style="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>546</v>
+      </c>
+      <c r="B1" s="19">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="B2" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>548</v>
+      </c>
+      <c r="B3" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>549</v>
+      </c>
+      <c r="B4" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>550</v>
+      </c>
+      <c r="B5" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>551</v>
+      </c>
+      <c r="B6" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>552</v>
+      </c>
+      <c r="B7" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>553</v>
+      </c>
+      <c r="B8" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>554</v>
+      </c>
+      <c r="B9" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>555</v>
+      </c>
+      <c r="B10" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>556</v>
+      </c>
+      <c r="B11" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>557</v>
+      </c>
+      <c r="B12" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
+        <v>558</v>
+      </c>
+      <c r="B13" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>559</v>
+      </c>
+      <c r="B14" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>560</v>
+      </c>
+      <c r="B15" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>561</v>
+      </c>
+      <c r="B16" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="B17" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>563</v>
+      </c>
+      <c r="B18" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>564</v>
+      </c>
+      <c r="B19" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>565</v>
+      </c>
+      <c r="B20" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
+        <v>566</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
+        <v>567</v>
+      </c>
+      <c r="B22" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>568</v>
+      </c>
+      <c r="B23" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
+        <v>569</v>
+      </c>
+      <c r="B24" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
+        <v>570</v>
+      </c>
+      <c r="B25" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="s">
+        <v>571</v>
+      </c>
+      <c r="B26" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
+        <v>572</v>
+      </c>
+      <c r="B27" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
+        <v>573</v>
+      </c>
+      <c r="B28" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>574</v>
+      </c>
+      <c r="B29" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
+        <v>575</v>
+      </c>
+      <c r="B30" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
+        <v>576</v>
+      </c>
+      <c r="B31" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="B32" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="20" t="s">
+        <v>578</v>
+      </c>
+      <c r="B33" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="20" t="s">
+        <v>579</v>
+      </c>
+      <c r="B34" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B35" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="20" t="s">
+        <v>581</v>
+      </c>
+      <c r="B36" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="20" t="s">
+        <v>582</v>
+      </c>
+      <c r="B37" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>583</v>
+      </c>
+      <c r="B38" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="20" t="s">
+        <v>584</v>
+      </c>
+      <c r="B39" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="20" t="s">
+        <v>585</v>
+      </c>
+      <c r="B40" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
+        <v>586</v>
+      </c>
+      <c r="B41" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="20" t="s">
+        <v>587</v>
+      </c>
+      <c r="B42" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="20" t="s">
+        <v>588</v>
+      </c>
+      <c r="B43" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="20" t="s">
+        <v>589</v>
+      </c>
+      <c r="B44" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="B45" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="20" t="s">
+        <v>591</v>
+      </c>
+      <c r="B46" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>592</v>
+      </c>
+      <c r="B47" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="B48" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="20" t="s">
+        <v>594</v>
+      </c>
+      <c r="B49" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="20" t="s">
+        <v>595</v>
+      </c>
+      <c r="B50" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
+        <v>596</v>
+      </c>
+      <c r="B51" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="20" t="s">
+        <v>597</v>
+      </c>
+      <c r="B52" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="B53" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="20" t="s">
+        <v>599</v>
+      </c>
+      <c r="B54" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="20" t="s">
+        <v>600</v>
+      </c>
+      <c r="B55" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="20" t="s">
+        <v>601</v>
+      </c>
+      <c r="B56" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="20" t="s">
+        <v>602</v>
+      </c>
+      <c r="B57" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="20" t="s">
+        <v>603</v>
+      </c>
+      <c r="B58" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="20" t="s">
+        <v>604</v>
+      </c>
+      <c r="B59" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="20" t="s">
+        <v>605</v>
+      </c>
+      <c r="B60" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="B61" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="20" t="s">
+        <v>607</v>
+      </c>
+      <c r="B62" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="20" t="s">
+        <v>608</v>
+      </c>
+      <c r="B63" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="20" t="s">
+        <v>609</v>
+      </c>
+      <c r="B64" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="20" t="s">
+        <v>610</v>
+      </c>
+      <c r="B65" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="20" t="s">
+        <v>611</v>
+      </c>
+      <c r="B66" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="20" t="s">
+        <v>612</v>
+      </c>
+      <c r="B67" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="20" t="s">
+        <v>613</v>
+      </c>
+      <c r="B68" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="20" t="s">
+        <v>614</v>
+      </c>
+      <c r="B69" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="20" t="s">
+        <v>615</v>
+      </c>
+      <c r="B70" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="20" t="s">
+        <v>616</v>
+      </c>
+      <c r="B71" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="20" t="s">
+        <v>617</v>
+      </c>
+      <c r="B72" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="20" t="s">
+        <v>618</v>
+      </c>
+      <c r="B73" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="20" t="s">
+        <v>619</v>
+      </c>
+      <c r="B74" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="20" t="s">
+        <v>620</v>
+      </c>
+      <c r="B75" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="20" t="s">
+        <v>621</v>
+      </c>
+      <c r="B76" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="20" t="s">
+        <v>622</v>
+      </c>
+      <c r="B77" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="20" t="s">
+        <v>623</v>
+      </c>
+      <c r="B78" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="20" t="s">
+        <v>624</v>
+      </c>
+      <c r="B79" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="20" t="s">
+        <v>625</v>
+      </c>
+      <c r="B80" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="20" t="s">
+        <v>626</v>
+      </c>
+      <c r="B81" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="20" t="s">
+        <v>627</v>
+      </c>
+      <c r="B82" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="20" t="s">
+        <v>628</v>
+      </c>
+      <c r="B83" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="20" t="s">
+        <v>629</v>
+      </c>
+      <c r="B84" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="20" t="s">
+        <v>630</v>
+      </c>
+      <c r="B85" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="20" t="s">
+        <v>631</v>
+      </c>
+      <c r="B86" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B87" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="20" t="s">
+        <v>632</v>
+      </c>
+      <c r="B88" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="B89" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="20" t="s">
+        <v>634</v>
+      </c>
+      <c r="B90" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="20" t="s">
+        <v>635</v>
+      </c>
+      <c r="B91" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="20" t="s">
+        <v>636</v>
+      </c>
+      <c r="B92" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" s="20" t="s">
+        <v>637</v>
+      </c>
+      <c r="B93" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" s="20" t="s">
+        <v>638</v>
+      </c>
+      <c r="B94" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" s="20" t="s">
+        <v>639</v>
+      </c>
+      <c r="B95" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="20" t="s">
+        <v>640</v>
+      </c>
+      <c r="B96" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="20" t="s">
+        <v>641</v>
+      </c>
+      <c r="B97" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="20" t="s">
+        <v>642</v>
+      </c>
+      <c r="B98" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="20" t="s">
+        <v>643</v>
+      </c>
+      <c r="B99" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="20" t="s">
+        <v>644</v>
+      </c>
+      <c r="B100" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="20" t="s">
+        <v>645</v>
+      </c>
+      <c r="B101" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="20" t="s">
+        <v>646</v>
+      </c>
+      <c r="B102" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="20" t="s">
+        <v>647</v>
+      </c>
+      <c r="B103" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="20" t="s">
+        <v>648</v>
+      </c>
+      <c r="B104" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="20" t="s">
+        <v>649</v>
+      </c>
+      <c r="B105" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="20" t="s">
+        <v>650</v>
+      </c>
+      <c r="B106" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="20" t="s">
+        <v>651</v>
+      </c>
+      <c r="B107" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="20" t="s">
+        <v>652</v>
+      </c>
+      <c r="B108" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" s="20" t="s">
+        <v>653</v>
+      </c>
+      <c r="B109" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" s="20" t="s">
+        <v>654</v>
+      </c>
+      <c r="B110" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="20" t="s">
+        <v>655</v>
+      </c>
+      <c r="B111" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="20" t="s">
+        <v>656</v>
+      </c>
+      <c r="B112" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="20" t="s">
+        <v>657</v>
+      </c>
+      <c r="B113" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="20" t="s">
+        <v>658</v>
+      </c>
+      <c r="B114" s="19">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F30D07-5DEA-784F-9379-3415E736F037}">
   <dimension ref="A1:AL49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>196</v>
       </c>
       <c r="B1">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>542</v>
       </c>
       <c r="E1" s="1"/>
@@ -5657,7 +6947,7 @@
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -5668,7 +6958,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>198</v>
       </c>
@@ -5679,7 +6969,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -5690,7 +6980,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>200</v>
       </c>
@@ -5701,7 +6991,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>201</v>
       </c>
@@ -5712,7 +7002,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>202</v>
       </c>
@@ -5723,7 +7013,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>203</v>
       </c>
@@ -5734,7 +7024,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>204</v>
       </c>
@@ -5745,7 +7035,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>205</v>
       </c>
@@ -5756,7 +7046,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>206</v>
       </c>
@@ -5767,7 +7057,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>207</v>
       </c>
@@ -5778,7 +7068,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>208</v>
       </c>
@@ -5789,7 +7079,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>209</v>
       </c>
@@ -5800,7 +7090,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>210</v>
       </c>
@@ -5811,7 +7101,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>211</v>
       </c>
@@ -5822,7 +7112,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>212</v>
       </c>
@@ -5833,7 +7123,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>213</v>
       </c>
@@ -5844,7 +7134,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>214</v>
       </c>
@@ -5855,7 +7145,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>215</v>
       </c>
@@ -5866,7 +7156,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>216</v>
       </c>
@@ -5877,7 +7167,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>217</v>
       </c>
@@ -5888,7 +7178,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>218</v>
       </c>
@@ -5899,7 +7189,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>219</v>
       </c>
@@ -5910,7 +7200,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>220</v>
       </c>
@@ -5921,7 +7211,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>221</v>
       </c>
@@ -5932,7 +7222,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>222</v>
       </c>
@@ -5943,7 +7233,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>223</v>
       </c>
@@ -5954,7 +7244,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>224</v>
       </c>
@@ -5965,7 +7255,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>225</v>
       </c>
@@ -5976,7 +7266,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>226</v>
       </c>
@@ -5987,7 +7277,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>227</v>
       </c>
@@ -5998,7 +7288,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>228</v>
       </c>
@@ -6009,7 +7299,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>229</v>
       </c>
@@ -6020,7 +7310,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>230</v>
       </c>
@@ -6031,7 +7321,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>231</v>
       </c>
@@ -6042,7 +7332,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>232</v>
       </c>
@@ -6053,7 +7343,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>233</v>
       </c>
@@ -6064,7 +7354,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>234</v>
       </c>
@@ -6075,7 +7365,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>235</v>
       </c>
@@ -6086,7 +7376,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>236</v>
       </c>
@@ -6097,7 +7387,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>237</v>
       </c>
@@ -6108,7 +7398,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>238</v>
       </c>
@@ -6119,7 +7409,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>239</v>
       </c>
@@ -6130,7 +7420,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>240</v>
       </c>
@@ -6141,7 +7431,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>241</v>
       </c>
@@ -6152,7 +7442,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>242</v>
       </c>
@@ -6163,7 +7453,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>280</v>
       </c>
@@ -6174,7 +7464,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>281</v>
       </c>
@@ -6417,6 +7707,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Notes xmlns="cf98b484-8438-4ffb-ac7b-f510e03aed50" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6425,22 +7723,39 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Notes xmlns="cf98b484-8438-4ffb-ac7b-f510e03aed50" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E134D722-4940-40C6-A5FC-5CC8501A7A3B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E134D722-4940-40C6-A5FC-5CC8501A7A3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cf98b484-8438-4ffb-ac7b-f510e03aed50"/>
+    <ds:schemaRef ds:uri="77ef6267-3d9c-46f3-8cdf-1b27c794ba93"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A850073-F096-40FE-9371-D09F388483C2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B29EF3-1851-4133-979D-D471BA3691DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cf98b484-8438-4ffb-ac7b-f510e03aed50"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B29EF3-1851-4133-979D-D471BA3691DC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A850073-F096-40FE-9371-D09F388483C2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>